<commit_message>
Fixed a big error. Products had incorrect getters now fixed. Made a test that works now. Will do more later today.
</commit_message>
<xml_diff>
--- a/PIM/src/test/java/files/linewithemptyrow.xlsx
+++ b/PIM/src/test/java/files/linewithemptyrow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frederik\Desktop\PIM\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frederik\Documents\GitHub\PIM\PIM\PIM\src\test\java\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95534DA-B3B6-47A3-9348-5287D94CD43E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDAF46C-DEC8-4B07-98E4-CA49DBB6B877}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{CCB885A0-B2BF-41E6-8454-AB292DEBF28F}"/>
   </bookViews>
@@ -62,22 +62,22 @@
     <t>No_picture_yet</t>
   </si>
   <si>
-    <t>Ærter (fine)</t>
-  </si>
-  <si>
-    <t>First Price</t>
-  </si>
-  <si>
     <t>ProductNameDescription</t>
   </si>
   <si>
-    <t>575 g / First Price</t>
-  </si>
-  <si>
-    <t>Grøntsager på frost</t>
-  </si>
-  <si>
     <t>Frost</t>
+  </si>
+  <si>
+    <t>Ispinde m. mandel</t>
+  </si>
+  <si>
+    <t>6 stk. / nemlig basic</t>
+  </si>
+  <si>
+    <t>NemligBasic</t>
+  </si>
+  <si>
+    <t>Is</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -485,32 +485,32 @@
     </row>
     <row r="2" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>9312</v>
+        <v>8337</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F2">
-        <v>9.5</v>
+        <v>29.95</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>